<commit_message>
post ops updates 2022
</commit_message>
<xml_diff>
--- a/static/download/2022/RP3_APT_ATFM_ARR_2022_Jan_Dec.xlsx
+++ b/static/download/2022/RP3_APT_ATFM_ARR_2022_Jan_Dec.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhegendo\repos\ses-portal\static\download\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhegendo\Downloads\01-release-20230526T152623Z-001\01-release\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD756A33-AEDE-463F-885F-C5F9F6443333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878C1FBD-8BFC-4F7A-8D03-721191073491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="55" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1363,106 +1363,89 @@
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FFF3F3F3"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="9"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -2152,7 +2135,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HEGENDORFER Holger" refreshedDate="45034.759665162041" refreshedVersion="8" recordCount="145" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="HEGENDORFER Holger" refreshedDate="45072.728279629628" refreshedVersion="8" recordCount="145" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A5:F150" sheet="APT_ATFM_APT"/>
   </cacheSource>
@@ -2318,17 +2301,17 @@
     <x v="1"/>
     <s v="Stuttgart (EDDS)"/>
     <s v="EDDS"/>
-    <n v="0.13608451290591175"/>
+    <n v="8.4877185678601169E-2"/>
     <n v="38432"/>
-    <n v="5230"/>
+    <n v="3262"/>
   </r>
   <r>
     <x v="1"/>
     <s v="Hanover (EDDV)"/>
     <s v="EDDV"/>
-    <n v="0.15932596291012838"/>
+    <n v="3.428138373751783E-2"/>
     <n v="22432"/>
-    <n v="3574"/>
+    <n v="769"/>
   </r>
   <r>
     <x v="1"/>
@@ -2630,9 +2613,9 @@
     <x v="12"/>
     <s v="Alicante (LEAL)"/>
     <s v="LEAL"/>
-    <n v="3.4510415506293864E-2"/>
+    <n v="3.096802940848836E-3"/>
     <n v="44885"/>
-    <n v="1549"/>
+    <n v="139"/>
   </r>
   <r>
     <x v="12"/>
@@ -3366,15 +3349,15 @@
     <x v="22"/>
     <s v="Zürich (LSZH)"/>
     <s v="LSZH"/>
-    <n v="0.57554686093769247"/>
+    <n v="0.92795361747681349"/>
     <n v="105557"/>
-    <n v="60753"/>
+    <n v="97952"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="APT_ATFM_LOC" cacheId="55" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="APT_ATFM_LOC" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" rowGrandTotals="0" compact="0" compactData="0">
   <location ref="A5:D29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField name="State" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
@@ -3853,7 +3836,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="8">
-        <v>45034</v>
+        <v>45072</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
@@ -4015,13 +3998,13 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>0.51451036940290051</v>
+        <v>0.52139739911154293</v>
       </c>
       <c r="C12" s="26">
         <v>4503538</v>
       </c>
       <c r="D12" s="26">
-        <v>2317117</v>
+        <v>2348133</v>
       </c>
       <c r="F12" s="21"/>
     </row>
@@ -4099,7 +4082,7 @@
       </c>
       <c r="B2" s="31">
         <f>APT_ATFM_SES_YY!B2</f>
-        <v>45034</v>
+        <v>45072</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
@@ -4959,17 +4942,17 @@
       </c>
       <c r="B42" s="56">
         <f t="shared" si="0"/>
-        <v>0.26972865083956188</v>
+        <v>0.27287772622965262</v>
       </c>
       <c r="C42" s="57">
         <v>261029</v>
       </c>
       <c r="D42" s="57">
-        <v>70407</v>
+        <v>71229</v>
       </c>
       <c r="E42" s="51">
         <f>D42/C42</f>
-        <v>0.26972865083956188</v>
+        <v>0.27287772622965262</v>
       </c>
       <c r="F42" s="61">
         <v>1</v>
@@ -4982,17 +4965,17 @@
       </c>
       <c r="B43" s="46">
         <f t="shared" si="0"/>
-        <v>0.20279120722093882</v>
+        <v>0.21131724975588845</v>
       </c>
       <c r="C43" s="26">
         <v>251934</v>
       </c>
       <c r="D43" s="26">
-        <v>51090</v>
+        <v>53238</v>
       </c>
       <c r="E43" s="48">
         <f t="shared" ref="E43:E53" si="3">SUM(D$42:D43)/SUM(C$42:C43)</f>
-        <v>0.23685334029939781</v>
+        <v>0.24264323157810602</v>
       </c>
       <c r="F43" s="62">
         <v>1</v>
@@ -5005,17 +4988,17 @@
       </c>
       <c r="B44" s="46">
         <f t="shared" si="0"/>
-        <v>9.7992332494861903E-2</v>
+        <v>9.8953102603407159E-2</v>
       </c>
       <c r="C44" s="26">
         <v>321617</v>
       </c>
       <c r="D44" s="26">
-        <v>31516</v>
+        <v>31825</v>
       </c>
       <c r="E44" s="48">
         <f t="shared" si="3"/>
-        <v>0.18334132138321071</v>
+        <v>0.18727024371540177</v>
       </c>
       <c r="F44" s="62">
         <v>1</v>
@@ -5028,17 +5011,17 @@
       </c>
       <c r="B45" s="46">
         <f t="shared" si="0"/>
-        <v>0.62049202760115951</v>
+        <v>0.62684231362973319</v>
       </c>
       <c r="C45" s="26">
         <v>376361</v>
       </c>
       <c r="D45" s="26">
-        <v>233529</v>
+        <v>235919</v>
       </c>
       <c r="E45" s="48">
         <f t="shared" si="3"/>
-        <v>0.31920795480539516</v>
+        <v>0.32388943804859194</v>
       </c>
       <c r="F45" s="62">
         <v>1</v>
@@ -5051,17 +5034,17 @@
       </c>
       <c r="B46" s="46">
         <f t="shared" si="0"/>
-        <v>0.50131862465674371</v>
+        <v>0.51459238532695983</v>
       </c>
       <c r="C46" s="26">
         <v>422789</v>
       </c>
       <c r="D46" s="26">
-        <v>211952</v>
+        <v>217564</v>
       </c>
       <c r="E46" s="48">
         <f t="shared" si="3"/>
-        <v>0.36633593066173725</v>
+        <v>0.37324098841301806</v>
       </c>
       <c r="F46" s="62">
         <v>1</v>
@@ -5074,17 +5057,17 @@
       </c>
       <c r="B47" s="46">
         <f t="shared" si="0"/>
-        <v>0.62844994433897339</v>
+        <v>0.64186402080475224</v>
       </c>
       <c r="C47" s="26">
         <v>432978</v>
       </c>
       <c r="D47" s="26">
-        <v>272105</v>
+        <v>277913</v>
       </c>
       <c r="E47" s="48">
         <f t="shared" si="3"/>
-        <v>0.42124915566204807</v>
+        <v>0.42951786125567809</v>
       </c>
       <c r="F47" s="62">
         <v>1</v>
@@ -5097,17 +5080,17 @@
       </c>
       <c r="B48" s="46">
         <f t="shared" si="0"/>
-        <v>0.58609649819018383</v>
+        <v>0.59055452588182422</v>
       </c>
       <c r="C48" s="26">
         <v>447283</v>
       </c>
       <c r="D48" s="26">
-        <v>262151</v>
+        <v>264145</v>
       </c>
       <c r="E48" s="48">
         <f t="shared" si="3"/>
-        <v>0.45057838313661425</v>
+        <v>0.45816910243513204</v>
       </c>
       <c r="F48" s="62">
         <v>1</v>
@@ -5120,17 +5103,17 @@
       </c>
       <c r="B49" s="46">
         <f t="shared" si="0"/>
-        <v>0.54457385167871186</v>
+        <v>0.55324503192642149</v>
       </c>
       <c r="C49" s="26">
         <v>446652</v>
       </c>
       <c r="D49" s="26">
-        <v>243235</v>
+        <v>247108</v>
       </c>
       <c r="E49" s="48">
         <f t="shared" si="3"/>
-        <v>0.46475883786055933</v>
+        <v>0.47251255892723304</v>
       </c>
       <c r="F49" s="62">
         <v>1</v>
@@ -5143,17 +5126,17 @@
       </c>
       <c r="B50" s="46">
         <f t="shared" si="0"/>
-        <v>0.53274279561661775</v>
+        <v>0.54442290001360294</v>
       </c>
       <c r="C50" s="26">
         <v>433729</v>
       </c>
       <c r="D50" s="26">
-        <v>231066</v>
+        <v>236132</v>
       </c>
       <c r="E50" s="48">
         <f t="shared" si="3"/>
-        <v>0.47344575078983681</v>
+        <v>0.48170118066022227</v>
       </c>
       <c r="F50" s="62">
         <v>1</v>
@@ -5166,17 +5149,17 @@
       </c>
       <c r="B51" s="46">
         <f t="shared" si="0"/>
-        <v>0.80607513611186565</v>
+        <v>0.80597120687822565</v>
       </c>
       <c r="C51" s="26">
         <v>423365</v>
       </c>
       <c r="D51" s="26">
-        <v>341264</v>
+        <v>341220</v>
       </c>
       <c r="E51" s="48">
         <f t="shared" si="3"/>
-        <v>0.51033242991856165</v>
+        <v>0.51766085510866777</v>
       </c>
       <c r="F51" s="62">
         <v>1</v>
@@ -5189,17 +5172,17 @@
       </c>
       <c r="B52" s="46">
         <f t="shared" si="0"/>
-        <v>0.5140352972360499</v>
+        <v>0.51687527125392863</v>
       </c>
       <c r="C52" s="26">
         <v>343313</v>
       </c>
       <c r="D52" s="26">
-        <v>176475</v>
+        <v>177450</v>
       </c>
       <c r="E52" s="48">
         <f t="shared" si="3"/>
-        <v>0.51063793994304318</v>
+        <v>0.5175960394611937</v>
       </c>
       <c r="F52" s="62">
         <v>1</v>
@@ -5212,17 +5195,17 @@
       </c>
       <c r="B53" s="46">
         <f t="shared" si="0"/>
-        <v>0.56155836116885849</v>
+        <v>0.56758192987783518</v>
       </c>
       <c r="C53" s="28">
         <v>342488</v>
       </c>
       <c r="D53" s="28">
-        <v>192327</v>
+        <v>194390</v>
       </c>
       <c r="E53" s="54">
         <f t="shared" si="3"/>
-        <v>0.51451036940290051</v>
+        <v>0.52139739911154293</v>
       </c>
       <c r="F53" s="60">
         <v>1</v>
@@ -5506,7 +5489,7 @@
   <dimension ref="A1:F530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5546,7 +5529,7 @@
       </c>
       <c r="B2" s="31">
         <f>APT_ATFM_SES_YY!B2</f>
-        <v>45034</v>
+        <v>45072</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
@@ -5755,11 +5738,11 @@
         <v>742813</v>
       </c>
       <c r="D14" s="103">
-        <v>213837</v>
+        <v>209064</v>
       </c>
       <c r="E14" s="69">
         <f t="shared" si="0"/>
-        <v>0.28787460639487999</v>
+        <v>0.28144903225980161</v>
       </c>
       <c r="F14" s="21"/>
     </row>
@@ -6004,11 +5987,11 @@
         <v>640765</v>
       </c>
       <c r="D27" s="103">
-        <v>311867</v>
+        <v>310457</v>
       </c>
       <c r="E27" s="69">
         <f t="shared" si="0"/>
-        <v>0.48671041645533075</v>
+        <v>0.48450992173417712</v>
       </c>
       <c r="F27" s="21"/>
     </row>
@@ -6042,11 +6025,11 @@
         <v>183379</v>
       </c>
       <c r="D29" s="107">
-        <v>98350</v>
+        <v>135549</v>
       </c>
       <c r="E29" s="69">
         <f t="shared" si="0"/>
-        <v>0.53632095278085279</v>
+        <v>0.73917406027953036</v>
       </c>
       <c r="F29" s="21"/>
     </row>
@@ -10109,7 +10092,7 @@
       </c>
       <c r="B2" s="31">
         <f>APT_ATFM_SES_YY!B2</f>
-        <v>45034</v>
+        <v>45072</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
@@ -10451,13 +10434,13 @@
       </c>
       <c r="D19" s="69">
         <f t="shared" si="0"/>
-        <v>0.13608451290591175</v>
+        <v>8.4877185678601169E-2</v>
       </c>
       <c r="E19" s="75">
         <v>38432</v>
       </c>
       <c r="F19" s="75">
-        <v>5230</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10472,13 +10455,13 @@
       </c>
       <c r="D20" s="69">
         <f t="shared" si="0"/>
-        <v>0.15932596291012838</v>
+        <v>3.428138373751783E-2</v>
       </c>
       <c r="E20" s="75">
         <v>22432</v>
       </c>
       <c r="F20" s="75">
-        <v>3574</v>
+        <v>769</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -11263,13 +11246,13 @@
       </c>
       <c r="D58" s="69">
         <f t="shared" si="1"/>
-        <v>3.4510415506293864E-2</v>
+        <v>3.096802940848836E-3</v>
       </c>
       <c r="E58" s="75">
         <v>44885</v>
       </c>
       <c r="F58" s="75">
-        <v>1549</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -13195,13 +13178,13 @@
       </c>
       <c r="D150" s="69">
         <f t="shared" si="1"/>
-        <v>0.57554686093769247</v>
+        <v>0.92795361747681349</v>
       </c>
       <c r="E150" s="75">
         <v>105557</v>
       </c>
       <c r="F150" s="75">
-        <v>60753</v>
+        <v>97952</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>